<commit_message>
Changed templates. updated the workflow processing to include REPEAT_STEP.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_Infinium_24_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_Infinium_24_v4_8_0.xlsx
@@ -25,7 +25,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>UFG</author>
   </authors>
   <commentList>
     <comment ref="B6" authorId="0">
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="481">
   <si>
     <t xml:space="preserve">Experiment Submission Template</t>
   </si>
@@ -488,13 +488,16 @@
     <t xml:space="preserve">A03</t>
   </si>
   <si>
-    <t xml:space="preserve">Ignore workflow - Do not register as part of a workflow</t>
+    <t xml:space="preserve">Repeat step - Move to next step and repeat current step</t>
   </si>
   <si>
     <t xml:space="preserve">B02</t>
   </si>
   <si>
     <t xml:space="preserve">A04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore workflow - Do not register as part of a workflow</t>
   </si>
   <si>
     <t xml:space="preserve">C01</t>
@@ -2107,7 +2110,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.43"/>
@@ -46190,7 +46193,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.86"/>
@@ -53550,7 +53553,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5:I100" type="list">
-      <formula1>Index!$F$2:$F$4</formula1>
+      <formula1>Index!$F$2:$F$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5:E100" type="none">
@@ -53579,7 +53582,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.53"/>
@@ -54060,7 +54063,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="16.43"/>
@@ -54154,265 +54157,268 @@
       <c r="E5" s="22" t="s">
         <v>101</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
       <c r="C14" s="22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>97</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="C15" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>100</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="22"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54420,7 +54426,7 @@
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E26" s="22" t="s">
         <v>97</v>
@@ -54431,7 +54437,7 @@
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>100</v>
@@ -54442,10 +54448,10 @@
       <c r="B28" s="22"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54453,10 +54459,10 @@
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54464,10 +54470,10 @@
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54475,10 +54481,10 @@
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54486,10 +54492,10 @@
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54497,10 +54503,10 @@
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54508,10 +54514,10 @@
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54519,10 +54525,10 @@
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54530,10 +54536,10 @@
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54541,10 +54547,10 @@
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54552,10 +54558,10 @@
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54563,10 +54569,10 @@
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54574,10 +54580,10 @@
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54585,10 +54591,10 @@
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54596,10 +54602,10 @@
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54607,10 +54613,10 @@
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54618,10 +54624,10 @@
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54629,10 +54635,10 @@
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54640,10 +54646,10 @@
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54651,10 +54657,10 @@
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54662,10 +54668,10 @@
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54673,10 +54679,10 @@
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54684,10 +54690,10 @@
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54695,10 +54701,10 @@
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54706,10 +54712,10 @@
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
       <c r="D52" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54717,10 +54723,10 @@
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
       <c r="D53" s="22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54728,10 +54734,10 @@
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54739,10 +54745,10 @@
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54750,10 +54756,10 @@
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
       <c r="D56" s="22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54761,10 +54767,10 @@
       <c r="B57" s="22"/>
       <c r="C57" s="22"/>
       <c r="D57" s="22" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54772,10 +54778,10 @@
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54783,10 +54789,10 @@
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54794,10 +54800,10 @@
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
       <c r="D60" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54805,10 +54811,10 @@
       <c r="B61" s="22"/>
       <c r="C61" s="22"/>
       <c r="D61" s="22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54816,10 +54822,10 @@
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
       <c r="D62" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54827,10 +54833,10 @@
       <c r="B63" s="22"/>
       <c r="C63" s="22"/>
       <c r="D63" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54838,10 +54844,10 @@
       <c r="B64" s="22"/>
       <c r="C64" s="22"/>
       <c r="D64" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54849,10 +54855,10 @@
       <c r="B65" s="22"/>
       <c r="C65" s="22"/>
       <c r="D65" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54860,10 +54866,10 @@
       <c r="B66" s="22"/>
       <c r="C66" s="22"/>
       <c r="D66" s="22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54871,10 +54877,10 @@
       <c r="B67" s="22"/>
       <c r="C67" s="22"/>
       <c r="D67" s="22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54882,10 +54888,10 @@
       <c r="B68" s="22"/>
       <c r="C68" s="22"/>
       <c r="D68" s="22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54893,10 +54899,10 @@
       <c r="B69" s="22"/>
       <c r="C69" s="22"/>
       <c r="D69" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54904,10 +54910,10 @@
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
       <c r="D70" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54915,10 +54921,10 @@
       <c r="B71" s="22"/>
       <c r="C71" s="22"/>
       <c r="D71" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54926,10 +54932,10 @@
       <c r="B72" s="22"/>
       <c r="C72" s="22"/>
       <c r="D72" s="22" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54937,10 +54943,10 @@
       <c r="B73" s="22"/>
       <c r="C73" s="22"/>
       <c r="D73" s="22" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E73" s="22" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54948,10 +54954,10 @@
       <c r="B74" s="22"/>
       <c r="C74" s="22"/>
       <c r="D74" s="22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54959,10 +54965,10 @@
       <c r="B75" s="22"/>
       <c r="C75" s="22"/>
       <c r="D75" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54970,10 +54976,10 @@
       <c r="B76" s="22"/>
       <c r="C76" s="22"/>
       <c r="D76" s="22" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54981,10 +54987,10 @@
       <c r="B77" s="22"/>
       <c r="C77" s="22"/>
       <c r="D77" s="22" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -54992,10 +54998,10 @@
       <c r="B78" s="22"/>
       <c r="C78" s="22"/>
       <c r="D78" s="22" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55003,10 +55009,10 @@
       <c r="B79" s="22"/>
       <c r="C79" s="22"/>
       <c r="D79" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E79" s="22" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55014,10 +55020,10 @@
       <c r="B80" s="22"/>
       <c r="C80" s="22"/>
       <c r="D80" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E80" s="22" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55025,10 +55031,10 @@
       <c r="B81" s="22"/>
       <c r="C81" s="22"/>
       <c r="D81" s="22" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55036,10 +55042,10 @@
       <c r="B82" s="22"/>
       <c r="C82" s="22"/>
       <c r="D82" s="22" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E82" s="22" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55047,10 +55053,10 @@
       <c r="B83" s="22"/>
       <c r="C83" s="22"/>
       <c r="D83" s="22" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55058,10 +55064,10 @@
       <c r="B84" s="22"/>
       <c r="C84" s="22"/>
       <c r="D84" s="22" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55069,10 +55075,10 @@
       <c r="B85" s="22"/>
       <c r="C85" s="22"/>
       <c r="D85" s="22" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55080,10 +55086,10 @@
       <c r="B86" s="22"/>
       <c r="C86" s="22"/>
       <c r="D86" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55091,10 +55097,10 @@
       <c r="B87" s="22"/>
       <c r="C87" s="22"/>
       <c r="D87" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E87" s="22" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55102,10 +55108,10 @@
       <c r="B88" s="22"/>
       <c r="C88" s="22"/>
       <c r="D88" s="22" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E88" s="22" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55113,10 +55119,10 @@
       <c r="B89" s="22"/>
       <c r="C89" s="22"/>
       <c r="D89" s="22" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E89" s="22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55124,10 +55130,10 @@
       <c r="B90" s="22"/>
       <c r="C90" s="22"/>
       <c r="D90" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E90" s="22" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55135,10 +55141,10 @@
       <c r="B91" s="22"/>
       <c r="C91" s="22"/>
       <c r="D91" s="22" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E91" s="22" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55146,10 +55152,10 @@
       <c r="B92" s="22"/>
       <c r="C92" s="22"/>
       <c r="D92" s="22" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E92" s="22" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55157,10 +55163,10 @@
       <c r="B93" s="22"/>
       <c r="C93" s="22"/>
       <c r="D93" s="22" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E93" s="22" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55168,10 +55174,10 @@
       <c r="B94" s="22"/>
       <c r="C94" s="22"/>
       <c r="D94" s="22" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E94" s="22" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55179,10 +55185,10 @@
       <c r="B95" s="22"/>
       <c r="C95" s="22"/>
       <c r="D95" s="22" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E95" s="22" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55190,10 +55196,10 @@
       <c r="B96" s="22"/>
       <c r="C96" s="22"/>
       <c r="D96" s="22" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E96" s="22" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55201,10 +55207,10 @@
       <c r="B97" s="22"/>
       <c r="C97" s="22"/>
       <c r="D97" s="22" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E97" s="22" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55213,7 +55219,7 @@
       <c r="C98" s="22"/>
       <c r="D98" s="22"/>
       <c r="E98" s="22" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55222,7 +55228,7 @@
       <c r="C99" s="22"/>
       <c r="D99" s="22"/>
       <c r="E99" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55231,7 +55237,7 @@
       <c r="C100" s="22"/>
       <c r="D100" s="22"/>
       <c r="E100" s="22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55240,7 +55246,7 @@
       <c r="C101" s="22"/>
       <c r="D101" s="22"/>
       <c r="E101" s="22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55249,7 +55255,7 @@
       <c r="C102" s="22"/>
       <c r="D102" s="22"/>
       <c r="E102" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55258,7 +55264,7 @@
       <c r="C103" s="22"/>
       <c r="D103" s="22"/>
       <c r="E103" s="22" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55267,7 +55273,7 @@
       <c r="C104" s="22"/>
       <c r="D104" s="22"/>
       <c r="E104" s="22" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55276,7 +55282,7 @@
       <c r="C105" s="22"/>
       <c r="D105" s="22"/>
       <c r="E105" s="22" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55285,7 +55291,7 @@
       <c r="C106" s="22"/>
       <c r="D106" s="22"/>
       <c r="E106" s="22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55294,7 +55300,7 @@
       <c r="C107" s="22"/>
       <c r="D107" s="22"/>
       <c r="E107" s="22" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55303,7 +55309,7 @@
       <c r="C108" s="22"/>
       <c r="D108" s="22"/>
       <c r="E108" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55312,7 +55318,7 @@
       <c r="C109" s="22"/>
       <c r="D109" s="22"/>
       <c r="E109" s="22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55321,7 +55327,7 @@
       <c r="C110" s="22"/>
       <c r="D110" s="22"/>
       <c r="E110" s="22" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55330,7 +55336,7 @@
       <c r="C111" s="22"/>
       <c r="D111" s="22"/>
       <c r="E111" s="22" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55339,7 +55345,7 @@
       <c r="C112" s="22"/>
       <c r="D112" s="22"/>
       <c r="E112" s="22" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55348,7 +55354,7 @@
       <c r="C113" s="22"/>
       <c r="D113" s="22"/>
       <c r="E113" s="22" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55357,7 +55363,7 @@
       <c r="C114" s="22"/>
       <c r="D114" s="22"/>
       <c r="E114" s="22" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55366,7 +55372,7 @@
       <c r="C115" s="22"/>
       <c r="D115" s="22"/>
       <c r="E115" s="22" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55375,7 +55381,7 @@
       <c r="C116" s="22"/>
       <c r="D116" s="22"/>
       <c r="E116" s="22" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55384,7 +55390,7 @@
       <c r="C117" s="22"/>
       <c r="D117" s="22"/>
       <c r="E117" s="22" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55393,7 +55399,7 @@
       <c r="C118" s="22"/>
       <c r="D118" s="22"/>
       <c r="E118" s="22" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55402,7 +55408,7 @@
       <c r="C119" s="22"/>
       <c r="D119" s="22"/>
       <c r="E119" s="22" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55411,7 +55417,7 @@
       <c r="C120" s="22"/>
       <c r="D120" s="22"/>
       <c r="E120" s="22" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55420,7 +55426,7 @@
       <c r="C121" s="22"/>
       <c r="D121" s="22"/>
       <c r="E121" s="22" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55429,7 +55435,7 @@
       <c r="C122" s="22"/>
       <c r="D122" s="22"/>
       <c r="E122" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55438,7 +55444,7 @@
       <c r="C123" s="22"/>
       <c r="D123" s="22"/>
       <c r="E123" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55447,7 +55453,7 @@
       <c r="C124" s="22"/>
       <c r="D124" s="22"/>
       <c r="E124" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55456,7 +55462,7 @@
       <c r="C125" s="22"/>
       <c r="D125" s="22"/>
       <c r="E125" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55465,7 +55471,7 @@
       <c r="C126" s="22"/>
       <c r="D126" s="22"/>
       <c r="E126" s="22" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55474,7 +55480,7 @@
       <c r="C127" s="22"/>
       <c r="D127" s="22"/>
       <c r="E127" s="22" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55483,7 +55489,7 @@
       <c r="C128" s="22"/>
       <c r="D128" s="22"/>
       <c r="E128" s="22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55492,7 +55498,7 @@
       <c r="C129" s="22"/>
       <c r="D129" s="22"/>
       <c r="E129" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55501,7 +55507,7 @@
       <c r="C130" s="22"/>
       <c r="D130" s="22"/>
       <c r="E130" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55510,7 +55516,7 @@
       <c r="C131" s="22"/>
       <c r="D131" s="22"/>
       <c r="E131" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55519,7 +55525,7 @@
       <c r="C132" s="22"/>
       <c r="D132" s="22"/>
       <c r="E132" s="22" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55528,7 +55534,7 @@
       <c r="C133" s="22"/>
       <c r="D133" s="22"/>
       <c r="E133" s="22" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55537,7 +55543,7 @@
       <c r="C134" s="22"/>
       <c r="D134" s="22"/>
       <c r="E134" s="22" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55546,7 +55552,7 @@
       <c r="C135" s="22"/>
       <c r="D135" s="22"/>
       <c r="E135" s="22" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55555,7 +55561,7 @@
       <c r="C136" s="22"/>
       <c r="D136" s="22"/>
       <c r="E136" s="22" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55564,7 +55570,7 @@
       <c r="C137" s="22"/>
       <c r="D137" s="22"/>
       <c r="E137" s="22" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55573,7 +55579,7 @@
       <c r="C138" s="22"/>
       <c r="D138" s="22"/>
       <c r="E138" s="22" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55582,7 +55588,7 @@
       <c r="C139" s="22"/>
       <c r="D139" s="22"/>
       <c r="E139" s="22" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55591,7 +55597,7 @@
       <c r="C140" s="22"/>
       <c r="D140" s="22"/>
       <c r="E140" s="22" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55600,7 +55606,7 @@
       <c r="C141" s="22"/>
       <c r="D141" s="22"/>
       <c r="E141" s="22" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55609,7 +55615,7 @@
       <c r="C142" s="22"/>
       <c r="D142" s="22"/>
       <c r="E142" s="22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55618,7 +55624,7 @@
       <c r="C143" s="22"/>
       <c r="D143" s="22"/>
       <c r="E143" s="22" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55627,7 +55633,7 @@
       <c r="C144" s="22"/>
       <c r="D144" s="22"/>
       <c r="E144" s="22" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55636,7 +55642,7 @@
       <c r="C145" s="22"/>
       <c r="D145" s="22"/>
       <c r="E145" s="22" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55645,7 +55651,7 @@
       <c r="C146" s="22"/>
       <c r="D146" s="22"/>
       <c r="E146" s="22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55654,7 +55660,7 @@
       <c r="C147" s="22"/>
       <c r="D147" s="22"/>
       <c r="E147" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55663,7 +55669,7 @@
       <c r="C148" s="22"/>
       <c r="D148" s="22"/>
       <c r="E148" s="22" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55672,7 +55678,7 @@
       <c r="C149" s="22"/>
       <c r="D149" s="22"/>
       <c r="E149" s="22" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55681,7 +55687,7 @@
       <c r="C150" s="22"/>
       <c r="D150" s="22"/>
       <c r="E150" s="22" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55690,7 +55696,7 @@
       <c r="C151" s="22"/>
       <c r="D151" s="22"/>
       <c r="E151" s="22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55699,7 +55705,7 @@
       <c r="C152" s="22"/>
       <c r="D152" s="22"/>
       <c r="E152" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55708,7 +55714,7 @@
       <c r="C153" s="22"/>
       <c r="D153" s="22"/>
       <c r="E153" s="22" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55717,7 +55723,7 @@
       <c r="C154" s="22"/>
       <c r="D154" s="22"/>
       <c r="E154" s="22" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55726,7 +55732,7 @@
       <c r="C155" s="22"/>
       <c r="D155" s="22"/>
       <c r="E155" s="22" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55735,7 +55741,7 @@
       <c r="C156" s="22"/>
       <c r="D156" s="22"/>
       <c r="E156" s="22" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55744,7 +55750,7 @@
       <c r="C157" s="22"/>
       <c r="D157" s="22"/>
       <c r="E157" s="22" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55753,7 +55759,7 @@
       <c r="C158" s="22"/>
       <c r="D158" s="22"/>
       <c r="E158" s="22" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55762,7 +55768,7 @@
       <c r="C159" s="22"/>
       <c r="D159" s="22"/>
       <c r="E159" s="22" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55771,7 +55777,7 @@
       <c r="C160" s="22"/>
       <c r="D160" s="22"/>
       <c r="E160" s="22" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55780,7 +55786,7 @@
       <c r="C161" s="22"/>
       <c r="D161" s="22"/>
       <c r="E161" s="22" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55789,7 +55795,7 @@
       <c r="C162" s="22"/>
       <c r="D162" s="22"/>
       <c r="E162" s="22" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55798,7 +55804,7 @@
       <c r="C163" s="22"/>
       <c r="D163" s="22"/>
       <c r="E163" s="22" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55807,7 +55813,7 @@
       <c r="C164" s="22"/>
       <c r="D164" s="22"/>
       <c r="E164" s="22" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55816,7 +55822,7 @@
       <c r="C165" s="22"/>
       <c r="D165" s="22"/>
       <c r="E165" s="22" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55825,7 +55831,7 @@
       <c r="C166" s="22"/>
       <c r="D166" s="22"/>
       <c r="E166" s="22" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55834,7 +55840,7 @@
       <c r="C167" s="22"/>
       <c r="D167" s="22"/>
       <c r="E167" s="22" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55843,7 +55849,7 @@
       <c r="C168" s="22"/>
       <c r="D168" s="22"/>
       <c r="E168" s="22" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55852,7 +55858,7 @@
       <c r="C169" s="22"/>
       <c r="D169" s="22"/>
       <c r="E169" s="22" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55861,7 +55867,7 @@
       <c r="C170" s="22"/>
       <c r="D170" s="22"/>
       <c r="E170" s="22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55870,7 +55876,7 @@
       <c r="C171" s="22"/>
       <c r="D171" s="22"/>
       <c r="E171" s="22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55879,7 +55885,7 @@
       <c r="C172" s="22"/>
       <c r="D172" s="22"/>
       <c r="E172" s="22" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55888,7 +55894,7 @@
       <c r="C173" s="22"/>
       <c r="D173" s="22"/>
       <c r="E173" s="22" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55897,7 +55903,7 @@
       <c r="C174" s="22"/>
       <c r="D174" s="22"/>
       <c r="E174" s="22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55906,7 +55912,7 @@
       <c r="C175" s="22"/>
       <c r="D175" s="22"/>
       <c r="E175" s="22" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55915,7 +55921,7 @@
       <c r="C176" s="22"/>
       <c r="D176" s="22"/>
       <c r="E176" s="22" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55924,7 +55930,7 @@
       <c r="C177" s="22"/>
       <c r="D177" s="22"/>
       <c r="E177" s="22" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55933,7 +55939,7 @@
       <c r="C178" s="22"/>
       <c r="D178" s="22"/>
       <c r="E178" s="22" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55942,7 +55948,7 @@
       <c r="C179" s="22"/>
       <c r="D179" s="22"/>
       <c r="E179" s="22" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55951,7 +55957,7 @@
       <c r="C180" s="22"/>
       <c r="D180" s="22"/>
       <c r="E180" s="22" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55960,7 +55966,7 @@
       <c r="C181" s="22"/>
       <c r="D181" s="22"/>
       <c r="E181" s="22" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55969,7 +55975,7 @@
       <c r="C182" s="22"/>
       <c r="D182" s="22"/>
       <c r="E182" s="22" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55978,7 +55984,7 @@
       <c r="C183" s="22"/>
       <c r="D183" s="22"/>
       <c r="E183" s="22" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55987,7 +55993,7 @@
       <c r="C184" s="22"/>
       <c r="D184" s="22"/>
       <c r="E184" s="22" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -55996,7 +56002,7 @@
       <c r="C185" s="22"/>
       <c r="D185" s="22"/>
       <c r="E185" s="22" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56005,7 +56011,7 @@
       <c r="C186" s="22"/>
       <c r="D186" s="22"/>
       <c r="E186" s="22" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56014,7 +56020,7 @@
       <c r="C187" s="22"/>
       <c r="D187" s="22"/>
       <c r="E187" s="22" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56023,7 +56029,7 @@
       <c r="C188" s="22"/>
       <c r="D188" s="22"/>
       <c r="E188" s="22" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56032,7 +56038,7 @@
       <c r="C189" s="22"/>
       <c r="D189" s="22"/>
       <c r="E189" s="22" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56041,7 +56047,7 @@
       <c r="C190" s="22"/>
       <c r="D190" s="22"/>
       <c r="E190" s="22" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56050,7 +56056,7 @@
       <c r="C191" s="22"/>
       <c r="D191" s="22"/>
       <c r="E191" s="22" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56059,7 +56065,7 @@
       <c r="C192" s="22"/>
       <c r="D192" s="22"/>
       <c r="E192" s="22" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56068,7 +56074,7 @@
       <c r="C193" s="22"/>
       <c r="D193" s="22"/>
       <c r="E193" s="22" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56077,7 +56083,7 @@
       <c r="C194" s="22"/>
       <c r="D194" s="22"/>
       <c r="E194" s="22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56086,7 +56092,7 @@
       <c r="C195" s="22"/>
       <c r="D195" s="22"/>
       <c r="E195" s="22" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56095,7 +56101,7 @@
       <c r="C196" s="22"/>
       <c r="D196" s="22"/>
       <c r="E196" s="22" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56104,7 +56110,7 @@
       <c r="C197" s="22"/>
       <c r="D197" s="22"/>
       <c r="E197" s="22" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56113,7 +56119,7 @@
       <c r="C198" s="22"/>
       <c r="D198" s="22"/>
       <c r="E198" s="22" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56122,7 +56128,7 @@
       <c r="C199" s="22"/>
       <c r="D199" s="22"/>
       <c r="E199" s="22" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56131,7 +56137,7 @@
       <c r="C200" s="22"/>
       <c r="D200" s="22"/>
       <c r="E200" s="22" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56140,7 +56146,7 @@
       <c r="C201" s="22"/>
       <c r="D201" s="22"/>
       <c r="E201" s="22" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56149,7 +56155,7 @@
       <c r="C202" s="22"/>
       <c r="D202" s="22"/>
       <c r="E202" s="22" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56158,7 +56164,7 @@
       <c r="C203" s="22"/>
       <c r="D203" s="22"/>
       <c r="E203" s="22" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56167,7 +56173,7 @@
       <c r="C204" s="22"/>
       <c r="D204" s="22"/>
       <c r="E204" s="22" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56176,7 +56182,7 @@
       <c r="C205" s="22"/>
       <c r="D205" s="22"/>
       <c r="E205" s="22" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56185,7 +56191,7 @@
       <c r="C206" s="22"/>
       <c r="D206" s="22"/>
       <c r="E206" s="22" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56194,7 +56200,7 @@
       <c r="C207" s="22"/>
       <c r="D207" s="22"/>
       <c r="E207" s="22" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56203,7 +56209,7 @@
       <c r="C208" s="22"/>
       <c r="D208" s="22"/>
       <c r="E208" s="22" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56212,7 +56218,7 @@
       <c r="C209" s="22"/>
       <c r="D209" s="22"/>
       <c r="E209" s="22" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56221,7 +56227,7 @@
       <c r="C210" s="22"/>
       <c r="D210" s="22"/>
       <c r="E210" s="22" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56230,7 +56236,7 @@
       <c r="C211" s="22"/>
       <c r="D211" s="22"/>
       <c r="E211" s="22" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56239,7 +56245,7 @@
       <c r="C212" s="22"/>
       <c r="D212" s="22"/>
       <c r="E212" s="22" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56248,7 +56254,7 @@
       <c r="C213" s="22"/>
       <c r="D213" s="22"/>
       <c r="E213" s="22" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56257,7 +56263,7 @@
       <c r="C214" s="22"/>
       <c r="D214" s="22"/>
       <c r="E214" s="22" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56266,7 +56272,7 @@
       <c r="C215" s="22"/>
       <c r="D215" s="22"/>
       <c r="E215" s="22" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56275,7 +56281,7 @@
       <c r="C216" s="22"/>
       <c r="D216" s="22"/>
       <c r="E216" s="22" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56284,7 +56290,7 @@
       <c r="C217" s="22"/>
       <c r="D217" s="22"/>
       <c r="E217" s="22" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56293,7 +56299,7 @@
       <c r="C218" s="22"/>
       <c r="D218" s="22"/>
       <c r="E218" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56302,7 +56308,7 @@
       <c r="C219" s="22"/>
       <c r="D219" s="22"/>
       <c r="E219" s="22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56311,7 +56317,7 @@
       <c r="C220" s="22"/>
       <c r="D220" s="22"/>
       <c r="E220" s="22" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56320,7 +56326,7 @@
       <c r="C221" s="22"/>
       <c r="D221" s="22"/>
       <c r="E221" s="22" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56329,7 +56335,7 @@
       <c r="C222" s="22"/>
       <c r="D222" s="22"/>
       <c r="E222" s="22" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56338,7 +56344,7 @@
       <c r="C223" s="22"/>
       <c r="D223" s="22"/>
       <c r="E223" s="22" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56347,7 +56353,7 @@
       <c r="C224" s="22"/>
       <c r="D224" s="22"/>
       <c r="E224" s="22" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56356,7 +56362,7 @@
       <c r="C225" s="22"/>
       <c r="D225" s="22"/>
       <c r="E225" s="22" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56365,7 +56371,7 @@
       <c r="C226" s="22"/>
       <c r="D226" s="22"/>
       <c r="E226" s="22" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56374,7 +56380,7 @@
       <c r="C227" s="22"/>
       <c r="D227" s="22"/>
       <c r="E227" s="22" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56383,7 +56389,7 @@
       <c r="C228" s="22"/>
       <c r="D228" s="22"/>
       <c r="E228" s="22" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56392,7 +56398,7 @@
       <c r="C229" s="22"/>
       <c r="D229" s="22"/>
       <c r="E229" s="22" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56401,7 +56407,7 @@
       <c r="C230" s="22"/>
       <c r="D230" s="22"/>
       <c r="E230" s="22" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56410,7 +56416,7 @@
       <c r="C231" s="22"/>
       <c r="D231" s="22"/>
       <c r="E231" s="22" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56419,7 +56425,7 @@
       <c r="C232" s="22"/>
       <c r="D232" s="22"/>
       <c r="E232" s="22" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56428,7 +56434,7 @@
       <c r="C233" s="22"/>
       <c r="D233" s="22"/>
       <c r="E233" s="22" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56437,7 +56443,7 @@
       <c r="C234" s="22"/>
       <c r="D234" s="22"/>
       <c r="E234" s="22" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56446,7 +56452,7 @@
       <c r="C235" s="22"/>
       <c r="D235" s="22"/>
       <c r="E235" s="22" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56455,7 +56461,7 @@
       <c r="C236" s="22"/>
       <c r="D236" s="22"/>
       <c r="E236" s="22" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56464,7 +56470,7 @@
       <c r="C237" s="22"/>
       <c r="D237" s="22"/>
       <c r="E237" s="22" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56473,7 +56479,7 @@
       <c r="C238" s="22"/>
       <c r="D238" s="22"/>
       <c r="E238" s="22" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56482,7 +56488,7 @@
       <c r="C239" s="22"/>
       <c r="D239" s="22"/>
       <c r="E239" s="22" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56491,7 +56497,7 @@
       <c r="C240" s="22"/>
       <c r="D240" s="22"/>
       <c r="E240" s="22" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56500,7 +56506,7 @@
       <c r="C241" s="22"/>
       <c r="D241" s="22"/>
       <c r="E241" s="22" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56509,7 +56515,7 @@
       <c r="C242" s="22"/>
       <c r="D242" s="22"/>
       <c r="E242" s="22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56518,7 +56524,7 @@
       <c r="C243" s="22"/>
       <c r="D243" s="22"/>
       <c r="E243" s="22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56527,7 +56533,7 @@
       <c r="C244" s="22"/>
       <c r="D244" s="22"/>
       <c r="E244" s="22" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56536,7 +56542,7 @@
       <c r="C245" s="22"/>
       <c r="D245" s="22"/>
       <c r="E245" s="22" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56545,7 +56551,7 @@
       <c r="C246" s="22"/>
       <c r="D246" s="22"/>
       <c r="E246" s="22" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56554,7 +56560,7 @@
       <c r="C247" s="22"/>
       <c r="D247" s="22"/>
       <c r="E247" s="22" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56563,7 +56569,7 @@
       <c r="C248" s="22"/>
       <c r="D248" s="22"/>
       <c r="E248" s="22" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56572,7 +56578,7 @@
       <c r="C249" s="22"/>
       <c r="D249" s="22"/>
       <c r="E249" s="22" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56581,7 +56587,7 @@
       <c r="C250" s="22"/>
       <c r="D250" s="22"/>
       <c r="E250" s="22" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56590,7 +56596,7 @@
       <c r="C251" s="22"/>
       <c r="D251" s="22"/>
       <c r="E251" s="22" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56599,7 +56605,7 @@
       <c r="C252" s="22"/>
       <c r="D252" s="22"/>
       <c r="E252" s="22" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56608,7 +56614,7 @@
       <c r="C253" s="22"/>
       <c r="D253" s="22"/>
       <c r="E253" s="22" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56617,7 +56623,7 @@
       <c r="C254" s="22"/>
       <c r="D254" s="22"/>
       <c r="E254" s="22" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56626,7 +56632,7 @@
       <c r="C255" s="22"/>
       <c r="D255" s="22"/>
       <c r="E255" s="22" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56635,7 +56641,7 @@
       <c r="C256" s="22"/>
       <c r="D256" s="22"/>
       <c r="E256" s="22" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56644,7 +56650,7 @@
       <c r="C257" s="22"/>
       <c r="D257" s="22"/>
       <c r="E257" s="22" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56653,7 +56659,7 @@
       <c r="C258" s="22"/>
       <c r="D258" s="22"/>
       <c r="E258" s="22" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56662,7 +56668,7 @@
       <c r="C259" s="22"/>
       <c r="D259" s="22"/>
       <c r="E259" s="22" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56671,7 +56677,7 @@
       <c r="C260" s="22"/>
       <c r="D260" s="22"/>
       <c r="E260" s="22" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56680,7 +56686,7 @@
       <c r="C261" s="22"/>
       <c r="D261" s="22"/>
       <c r="E261" s="22" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56689,7 +56695,7 @@
       <c r="C262" s="22"/>
       <c r="D262" s="22"/>
       <c r="E262" s="22" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56698,7 +56704,7 @@
       <c r="C263" s="22"/>
       <c r="D263" s="22"/>
       <c r="E263" s="22" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56707,7 +56713,7 @@
       <c r="C264" s="22"/>
       <c r="D264" s="22"/>
       <c r="E264" s="22" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56716,7 +56722,7 @@
       <c r="C265" s="22"/>
       <c r="D265" s="22"/>
       <c r="E265" s="22" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56725,7 +56731,7 @@
       <c r="C266" s="22"/>
       <c r="D266" s="22"/>
       <c r="E266" s="22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56734,7 +56740,7 @@
       <c r="C267" s="22"/>
       <c r="D267" s="22"/>
       <c r="E267" s="22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56743,7 +56749,7 @@
       <c r="C268" s="22"/>
       <c r="D268" s="22"/>
       <c r="E268" s="22" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56752,7 +56758,7 @@
       <c r="C269" s="22"/>
       <c r="D269" s="22"/>
       <c r="E269" s="22" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56761,7 +56767,7 @@
       <c r="C270" s="22"/>
       <c r="D270" s="22"/>
       <c r="E270" s="22" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56770,7 +56776,7 @@
       <c r="C271" s="22"/>
       <c r="D271" s="22"/>
       <c r="E271" s="22" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56779,7 +56785,7 @@
       <c r="C272" s="22"/>
       <c r="D272" s="22"/>
       <c r="E272" s="22" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56788,7 +56794,7 @@
       <c r="C273" s="22"/>
       <c r="D273" s="22"/>
       <c r="E273" s="22" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56797,7 +56803,7 @@
       <c r="C274" s="22"/>
       <c r="D274" s="22"/>
       <c r="E274" s="22" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56806,7 +56812,7 @@
       <c r="C275" s="22"/>
       <c r="D275" s="22"/>
       <c r="E275" s="22" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56815,7 +56821,7 @@
       <c r="C276" s="22"/>
       <c r="D276" s="22"/>
       <c r="E276" s="22" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56824,7 +56830,7 @@
       <c r="C277" s="22"/>
       <c r="D277" s="22"/>
       <c r="E277" s="22" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56833,7 +56839,7 @@
       <c r="C278" s="22"/>
       <c r="D278" s="22"/>
       <c r="E278" s="22" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56842,7 +56848,7 @@
       <c r="C279" s="22"/>
       <c r="D279" s="22"/>
       <c r="E279" s="22" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56851,7 +56857,7 @@
       <c r="C280" s="22"/>
       <c r="D280" s="22"/>
       <c r="E280" s="22" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56860,7 +56866,7 @@
       <c r="C281" s="22"/>
       <c r="D281" s="22"/>
       <c r="E281" s="22" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56869,7 +56875,7 @@
       <c r="C282" s="22"/>
       <c r="D282" s="22"/>
       <c r="E282" s="22" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56878,7 +56884,7 @@
       <c r="C283" s="22"/>
       <c r="D283" s="22"/>
       <c r="E283" s="22" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56887,7 +56893,7 @@
       <c r="C284" s="22"/>
       <c r="D284" s="22"/>
       <c r="E284" s="22" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56896,7 +56902,7 @@
       <c r="C285" s="22"/>
       <c r="D285" s="22"/>
       <c r="E285" s="22" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56905,7 +56911,7 @@
       <c r="C286" s="22"/>
       <c r="D286" s="22"/>
       <c r="E286" s="22" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56914,7 +56920,7 @@
       <c r="C287" s="22"/>
       <c r="D287" s="22"/>
       <c r="E287" s="22" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56923,7 +56929,7 @@
       <c r="C288" s="22"/>
       <c r="D288" s="22"/>
       <c r="E288" s="22" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56932,7 +56938,7 @@
       <c r="C289" s="22"/>
       <c r="D289" s="22"/>
       <c r="E289" s="22" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56941,7 +56947,7 @@
       <c r="C290" s="22"/>
       <c r="D290" s="22"/>
       <c r="E290" s="22" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56950,7 +56956,7 @@
       <c r="C291" s="22"/>
       <c r="D291" s="22"/>
       <c r="E291" s="22" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56959,7 +56965,7 @@
       <c r="C292" s="22"/>
       <c r="D292" s="22"/>
       <c r="E292" s="22" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56968,7 +56974,7 @@
       <c r="C293" s="22"/>
       <c r="D293" s="22"/>
       <c r="E293" s="22" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56977,7 +56983,7 @@
       <c r="C294" s="22"/>
       <c r="D294" s="22"/>
       <c r="E294" s="22" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56986,7 +56992,7 @@
       <c r="C295" s="22"/>
       <c r="D295" s="22"/>
       <c r="E295" s="22" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -56995,7 +57001,7 @@
       <c r="C296" s="22"/>
       <c r="D296" s="22"/>
       <c r="E296" s="22" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57004,7 +57010,7 @@
       <c r="C297" s="22"/>
       <c r="D297" s="22"/>
       <c r="E297" s="22" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57013,7 +57019,7 @@
       <c r="C298" s="22"/>
       <c r="D298" s="22"/>
       <c r="E298" s="22" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57022,7 +57028,7 @@
       <c r="C299" s="22"/>
       <c r="D299" s="22"/>
       <c r="E299" s="22" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57031,7 +57037,7 @@
       <c r="C300" s="22"/>
       <c r="D300" s="22"/>
       <c r="E300" s="22" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57040,7 +57046,7 @@
       <c r="C301" s="22"/>
       <c r="D301" s="22"/>
       <c r="E301" s="22" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57049,7 +57055,7 @@
       <c r="C302" s="22"/>
       <c r="D302" s="22"/>
       <c r="E302" s="22" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57058,7 +57064,7 @@
       <c r="C303" s="22"/>
       <c r="D303" s="22"/>
       <c r="E303" s="22" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57067,7 +57073,7 @@
       <c r="C304" s="22"/>
       <c r="D304" s="22"/>
       <c r="E304" s="22" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57076,7 +57082,7 @@
       <c r="C305" s="22"/>
       <c r="D305" s="22"/>
       <c r="E305" s="22" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57085,7 +57091,7 @@
       <c r="C306" s="22"/>
       <c r="D306" s="22"/>
       <c r="E306" s="22" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57094,7 +57100,7 @@
       <c r="C307" s="22"/>
       <c r="D307" s="22"/>
       <c r="E307" s="22" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57103,7 +57109,7 @@
       <c r="C308" s="22"/>
       <c r="D308" s="22"/>
       <c r="E308" s="22" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57112,7 +57118,7 @@
       <c r="C309" s="22"/>
       <c r="D309" s="22"/>
       <c r="E309" s="22" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57121,7 +57127,7 @@
       <c r="C310" s="22"/>
       <c r="D310" s="22"/>
       <c r="E310" s="22" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57130,7 +57136,7 @@
       <c r="C311" s="22"/>
       <c r="D311" s="22"/>
       <c r="E311" s="22" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57139,7 +57145,7 @@
       <c r="C312" s="22"/>
       <c r="D312" s="22"/>
       <c r="E312" s="22" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57148,7 +57154,7 @@
       <c r="C313" s="22"/>
       <c r="D313" s="22"/>
       <c r="E313" s="22" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57157,7 +57163,7 @@
       <c r="C314" s="22"/>
       <c r="D314" s="22"/>
       <c r="E314" s="22" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57166,7 +57172,7 @@
       <c r="C315" s="22"/>
       <c r="D315" s="22"/>
       <c r="E315" s="22" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57175,7 +57181,7 @@
       <c r="C316" s="22"/>
       <c r="D316" s="22"/>
       <c r="E316" s="22" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57184,7 +57190,7 @@
       <c r="C317" s="22"/>
       <c r="D317" s="22"/>
       <c r="E317" s="22" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57193,7 +57199,7 @@
       <c r="C318" s="22"/>
       <c r="D318" s="22"/>
       <c r="E318" s="22" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57202,7 +57208,7 @@
       <c r="C319" s="22"/>
       <c r="D319" s="22"/>
       <c r="E319" s="22" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57211,7 +57217,7 @@
       <c r="C320" s="22"/>
       <c r="D320" s="22"/>
       <c r="E320" s="22" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57220,7 +57226,7 @@
       <c r="C321" s="22"/>
       <c r="D321" s="22"/>
       <c r="E321" s="22" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57229,7 +57235,7 @@
       <c r="C322" s="22"/>
       <c r="D322" s="22"/>
       <c r="E322" s="22" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57238,7 +57244,7 @@
       <c r="C323" s="22"/>
       <c r="D323" s="22"/>
       <c r="E323" s="22" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57247,7 +57253,7 @@
       <c r="C324" s="22"/>
       <c r="D324" s="22"/>
       <c r="E324" s="22" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57256,7 +57262,7 @@
       <c r="C325" s="22"/>
       <c r="D325" s="22"/>
       <c r="E325" s="22" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57265,7 +57271,7 @@
       <c r="C326" s="22"/>
       <c r="D326" s="22"/>
       <c r="E326" s="22" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57274,7 +57280,7 @@
       <c r="C327" s="22"/>
       <c r="D327" s="22"/>
       <c r="E327" s="22" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57283,7 +57289,7 @@
       <c r="C328" s="22"/>
       <c r="D328" s="22"/>
       <c r="E328" s="22" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57292,7 +57298,7 @@
       <c r="C329" s="22"/>
       <c r="D329" s="22"/>
       <c r="E329" s="22" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57301,7 +57307,7 @@
       <c r="C330" s="22"/>
       <c r="D330" s="22"/>
       <c r="E330" s="22" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57310,7 +57316,7 @@
       <c r="C331" s="22"/>
       <c r="D331" s="22"/>
       <c r="E331" s="22" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57319,7 +57325,7 @@
       <c r="C332" s="22"/>
       <c r="D332" s="22"/>
       <c r="E332" s="22" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57328,7 +57334,7 @@
       <c r="C333" s="22"/>
       <c r="D333" s="22"/>
       <c r="E333" s="22" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57337,7 +57343,7 @@
       <c r="C334" s="22"/>
       <c r="D334" s="22"/>
       <c r="E334" s="22" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57346,7 +57352,7 @@
       <c r="C335" s="22"/>
       <c r="D335" s="22"/>
       <c r="E335" s="22" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57355,7 +57361,7 @@
       <c r="C336" s="22"/>
       <c r="D336" s="22"/>
       <c r="E336" s="22" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57364,7 +57370,7 @@
       <c r="C337" s="22"/>
       <c r="D337" s="22"/>
       <c r="E337" s="22" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57373,7 +57379,7 @@
       <c r="C338" s="22"/>
       <c r="D338" s="22"/>
       <c r="E338" s="22" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57382,7 +57388,7 @@
       <c r="C339" s="22"/>
       <c r="D339" s="22"/>
       <c r="E339" s="22" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57391,7 +57397,7 @@
       <c r="C340" s="22"/>
       <c r="D340" s="22"/>
       <c r="E340" s="22" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57400,7 +57406,7 @@
       <c r="C341" s="22"/>
       <c r="D341" s="22"/>
       <c r="E341" s="22" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57409,7 +57415,7 @@
       <c r="C342" s="22"/>
       <c r="D342" s="22"/>
       <c r="E342" s="22" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57418,7 +57424,7 @@
       <c r="C343" s="22"/>
       <c r="D343" s="22"/>
       <c r="E343" s="22" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57427,7 +57433,7 @@
       <c r="C344" s="22"/>
       <c r="D344" s="22"/>
       <c r="E344" s="22" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57436,7 +57442,7 @@
       <c r="C345" s="22"/>
       <c r="D345" s="22"/>
       <c r="E345" s="22" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57445,7 +57451,7 @@
       <c r="C346" s="22"/>
       <c r="D346" s="22"/>
       <c r="E346" s="22" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57454,7 +57460,7 @@
       <c r="C347" s="22"/>
       <c r="D347" s="22"/>
       <c r="E347" s="22" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57463,7 +57469,7 @@
       <c r="C348" s="22"/>
       <c r="D348" s="22"/>
       <c r="E348" s="22" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57472,7 +57478,7 @@
       <c r="C349" s="22"/>
       <c r="D349" s="22"/>
       <c r="E349" s="22" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57481,7 +57487,7 @@
       <c r="C350" s="22"/>
       <c r="D350" s="22"/>
       <c r="E350" s="22" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57490,7 +57496,7 @@
       <c r="C351" s="22"/>
       <c r="D351" s="22"/>
       <c r="E351" s="22" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57499,7 +57505,7 @@
       <c r="C352" s="22"/>
       <c r="D352" s="22"/>
       <c r="E352" s="22" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57508,7 +57514,7 @@
       <c r="C353" s="22"/>
       <c r="D353" s="22"/>
       <c r="E353" s="22" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57517,7 +57523,7 @@
       <c r="C354" s="22"/>
       <c r="D354" s="22"/>
       <c r="E354" s="22" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57526,7 +57532,7 @@
       <c r="C355" s="22"/>
       <c r="D355" s="22"/>
       <c r="E355" s="22" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57535,7 +57541,7 @@
       <c r="C356" s="22"/>
       <c r="D356" s="22"/>
       <c r="E356" s="22" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57544,7 +57550,7 @@
       <c r="C357" s="22"/>
       <c r="D357" s="22"/>
       <c r="E357" s="22" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57553,7 +57559,7 @@
       <c r="C358" s="22"/>
       <c r="D358" s="22"/>
       <c r="E358" s="22" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57562,7 +57568,7 @@
       <c r="C359" s="22"/>
       <c r="D359" s="22"/>
       <c r="E359" s="22" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57571,7 +57577,7 @@
       <c r="C360" s="22"/>
       <c r="D360" s="22"/>
       <c r="E360" s="22" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57580,7 +57586,7 @@
       <c r="C361" s="22"/>
       <c r="D361" s="22"/>
       <c r="E361" s="22" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57589,7 +57595,7 @@
       <c r="C362" s="22"/>
       <c r="D362" s="22"/>
       <c r="E362" s="22" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57598,7 +57604,7 @@
       <c r="C363" s="22"/>
       <c r="D363" s="22"/>
       <c r="E363" s="22" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57607,7 +57613,7 @@
       <c r="C364" s="22"/>
       <c r="D364" s="22"/>
       <c r="E364" s="22" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57616,7 +57622,7 @@
       <c r="C365" s="22"/>
       <c r="D365" s="22"/>
       <c r="E365" s="22" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57625,7 +57631,7 @@
       <c r="C366" s="22"/>
       <c r="D366" s="22"/>
       <c r="E366" s="22" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57634,7 +57640,7 @@
       <c r="C367" s="22"/>
       <c r="D367" s="22"/>
       <c r="E367" s="22" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57643,7 +57649,7 @@
       <c r="C368" s="22"/>
       <c r="D368" s="22"/>
       <c r="E368" s="22" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57652,7 +57658,7 @@
       <c r="C369" s="22"/>
       <c r="D369" s="22"/>
       <c r="E369" s="22" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57661,7 +57667,7 @@
       <c r="C370" s="22"/>
       <c r="D370" s="22"/>
       <c r="E370" s="22" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57670,7 +57676,7 @@
       <c r="C371" s="22"/>
       <c r="D371" s="22"/>
       <c r="E371" s="22" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57679,7 +57685,7 @@
       <c r="C372" s="22"/>
       <c r="D372" s="22"/>
       <c r="E372" s="22" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57688,7 +57694,7 @@
       <c r="C373" s="22"/>
       <c r="D373" s="22"/>
       <c r="E373" s="22" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57697,7 +57703,7 @@
       <c r="C374" s="22"/>
       <c r="D374" s="22"/>
       <c r="E374" s="22" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57706,7 +57712,7 @@
       <c r="C375" s="22"/>
       <c r="D375" s="22"/>
       <c r="E375" s="22" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57715,7 +57721,7 @@
       <c r="C376" s="22"/>
       <c r="D376" s="22"/>
       <c r="E376" s="22" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57724,7 +57730,7 @@
       <c r="C377" s="22"/>
       <c r="D377" s="22"/>
       <c r="E377" s="22" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57733,7 +57739,7 @@
       <c r="C378" s="22"/>
       <c r="D378" s="22"/>
       <c r="E378" s="22" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57742,7 +57748,7 @@
       <c r="C379" s="22"/>
       <c r="D379" s="22"/>
       <c r="E379" s="22" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57751,7 +57757,7 @@
       <c r="C380" s="22"/>
       <c r="D380" s="22"/>
       <c r="E380" s="22" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57760,7 +57766,7 @@
       <c r="C381" s="22"/>
       <c r="D381" s="22"/>
       <c r="E381" s="22" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57769,7 +57775,7 @@
       <c r="C382" s="22"/>
       <c r="D382" s="22"/>
       <c r="E382" s="22" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57778,7 +57784,7 @@
       <c r="C383" s="22"/>
       <c r="D383" s="22"/>
       <c r="E383" s="22" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57787,7 +57793,7 @@
       <c r="C384" s="22"/>
       <c r="D384" s="22"/>
       <c r="E384" s="22" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -57796,7 +57802,7 @@
       <c r="C385" s="22"/>
       <c r="D385" s="22"/>
       <c r="E385" s="22" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>